<commit_message>
Added Priority to Login&Queue
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData1.xlsx
+++ b/src/test/resources/testdata/TestData1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1B56975D-E12E-472A-96E8-E5363E33EA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{766A609B-C62B-4472-A215-219C8312153B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" tabRatio="500" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default_LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Graph" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F9"/>
+  <oleSize ref="A1:F7"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="58">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t xml:space="preserve">Missing username and  password </t>
-  </si>
-  <si>
-    <t>Please fill out this field</t>
   </si>
   <si>
     <t xml:space="preserve">Missing username </t>
@@ -794,32 +791,32 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
         <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -836,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -865,57 +862,57 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -948,32 +945,32 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1005,48 +1002,48 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>321</v>
@@ -1066,7 +1063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1078,32 +1075,32 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1132,32 +1129,32 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1197,121 +1194,121 @@
         <v>7</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="C9" s="8">
         <v>123456789</v>
@@ -1320,7 +1317,7 @@
         <v>123456789</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1352,32 +1349,32 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
         <v>54</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>55</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1406,32 +1403,32 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
         <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>